<commit_message>
Making gdml load and write symmetric
</commit_message>
<xml_diff>
--- a/pyg4ometry/test/Test.xlsx
+++ b/pyg4ometry/test/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sboogert/Dropbox (Royal Holloway)/Physics/coderepos/pyg4ometry/pyg4ometry/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38183AB7-BFD9-A249-B0CF-053933D366F2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B2ABB2-31F8-B24F-9647-FC3B4D6BA82C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="1340" windowWidth="28040" windowHeight="17440" xr2:uid="{BE135B9E-B31C-574F-8592-D8240EC2EAB0}"/>
+    <workbookView xWindow="3040" yWindow="1340" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{BE135B9E-B31C-574F-8592-D8240EC2EAB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Solids" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t xml:space="preserve">Solid </t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Assembly</t>
+  </si>
+  <si>
+    <t>Reflection</t>
+  </si>
+  <si>
+    <t>Optical</t>
   </si>
 </sst>
 </file>
@@ -465,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DC8304-9604-F142-A8F4-B5FD30AD7F5A}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView zoomScale="114" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,7 +573,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -608,10 +614,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7012F11D-CF3F-5448-8158-AC74577E7964}">
-  <dimension ref="A2:A5"/>
+  <dimension ref="A2:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -636,6 +642,16 @@
         <v>22</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Noted the completed GDML loading tests
</commit_message>
<xml_diff>
--- a/pyg4ometry/test/Test.xlsx
+++ b/pyg4ometry/test/Test.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sboogert/Dropbox (Royal Holloway)/Physics/coderepos/pyg4ometry/pyg4ometry/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aabramov/physics/coderepos/pyg4ometry/pyg4ometry/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B2ABB2-31F8-B24F-9647-FC3B4D6BA82C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="1340" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{BE135B9E-B31C-574F-8592-D8240EC2EAB0}"/>
+    <workbookView xWindow="3040" yWindow="1340" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="Solids" sheetId="1" r:id="rId1"/>
@@ -18,9 +17,15 @@
     <sheet name="Descriptions" sheetId="2" r:id="rId3"/>
     <sheet name="Other" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
   <si>
     <t xml:space="preserve">Solid </t>
   </si>
@@ -99,9 +104,6 @@
     <t>Auxilary information</t>
   </si>
   <si>
-    <t>multiunion</t>
-  </si>
-  <si>
     <t>Assembly</t>
   </si>
   <si>
@@ -109,12 +111,108 @@
   </si>
   <si>
     <t>Optical</t>
+  </si>
+  <si>
+    <t>Tube</t>
+  </si>
+  <si>
+    <t>Cut Tube</t>
+  </si>
+  <si>
+    <t>Cone</t>
+  </si>
+  <si>
+    <t>Para</t>
+  </si>
+  <si>
+    <t>Trd</t>
+  </si>
+  <si>
+    <t>Trap</t>
+  </si>
+  <si>
+    <t>Sphere</t>
+  </si>
+  <si>
+    <t>Orb</t>
+  </si>
+  <si>
+    <t>Torus</t>
+  </si>
+  <si>
+    <t>Polycone</t>
+  </si>
+  <si>
+    <t>Polyhedra</t>
+  </si>
+  <si>
+    <t>Ellipical Tube</t>
+  </si>
+  <si>
+    <t>Ellipsoid</t>
+  </si>
+  <si>
+    <t>Paraboloid</t>
+  </si>
+  <si>
+    <t>Multiunion</t>
+  </si>
+  <si>
+    <t>Hype</t>
+  </si>
+  <si>
+    <t>Tet</t>
+  </si>
+  <si>
+    <t>Extrusion solid</t>
+  </si>
+  <si>
+    <t>Twisted box</t>
+  </si>
+  <si>
+    <t>Elliptical cone</t>
+  </si>
+  <si>
+    <t>Generic polycone</t>
+  </si>
+  <si>
+    <t>Generic polyhedra</t>
+  </si>
+  <si>
+    <t>Twisted trap</t>
+  </si>
+  <si>
+    <t>Twisted trd</t>
+  </si>
+  <si>
+    <t>Arbitrary trap</t>
+  </si>
+  <si>
+    <t>Tessellated solid</t>
+  </si>
+  <si>
+    <t>Union</t>
+  </si>
+  <si>
+    <t>Subtraction</t>
+  </si>
+  <si>
+    <t>Intersection</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total solids</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -152,9 +250,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,15 +572,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DC8304-9604-F142-A8F4-B5FD30AD7F5A}">
-  <dimension ref="A1:D21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView zoomScale="114" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
@@ -500,11 +605,249 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>21</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="2">
+        <f>COUNTA(B2:B31)</f>
+        <v>19</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" ref="C32:D32" si="0">COUNTA(C2:C31)</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="3">
+        <f>COUNTBLANK(B1:B31) + COUNTA(B2:B31)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -512,7 +855,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6710EEAB-41DD-5141-849B-39D8768237C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -521,6 +864,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
@@ -569,7 +913,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2877E0A3-C0FC-9B46-9AF7-22787A2B833F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -613,14 +957,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7012F11D-CF3F-5448-8158-AC74577E7964}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -639,17 +986,17 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Python authoring unit tests
</commit_message>
<xml_diff>
--- a/pyg4ometry/test/Test.xlsx
+++ b/pyg4ometry/test/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sboogert/Dropbox (Royal Holloway)/Physics/coderepos/pyg4ometry/pyg4ometry/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B2ABB2-31F8-B24F-9647-FC3B4D6BA82C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FC5610-88CB-E940-9EE3-CA75477CCAF6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="1340" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{BE135B9E-B31C-574F-8592-D8240EC2EAB0}"/>
+    <workbookView xWindow="13220" yWindow="1120" windowWidth="28040" windowHeight="17440" xr2:uid="{BE135B9E-B31C-574F-8592-D8240EC2EAB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Solids" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t xml:space="preserve">Solid </t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Optical</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -152,9 +155,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DC8304-9604-F142-A8F4-B5FD30AD7F5A}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView zoomScale="114" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -483,28 +492,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -616,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7012F11D-CF3F-5448-8158-AC74577E7964}">
   <dimension ref="A2:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>